<commit_message>
Manually updated some data
</commit_message>
<xml_diff>
--- a/Data Collection/Authors/Annemarie Piper/articles_Piper_Jan_1.xlsx
+++ b/Data Collection/Authors/Annemarie Piper/articles_Piper_Jan_1.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c6ad9d82f21af58/Dokumente/COINS_SwissTribeleaders/Data Collection/Authors/Annemarie Piper/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_B3DFE4B0F48EEABE219C86F2624B05D92B17A793" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1FAB00A9-01BA-4DF6-BD1B-3501A7FFD4A6}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>title</t>
   </si>
@@ -25,18 +31,12 @@
     <t>date</t>
   </si>
   <si>
-    <t>datetime</t>
-  </si>
-  <si>
     <t>desc</t>
   </si>
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>img</t>
-  </si>
-  <si>
     <t>summary</t>
   </si>
   <si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>https://www.ndr.de/kultur/buch/Lionel-Shriver-Die-perfekte-Freundin,perfektefreundin102.html</t>
-  </si>
-  <si>
-    <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///////yH5BAEKAAEALAAAAAABAAEAAAICTAEAOw==</t>
   </si>
   <si>
     <t>Annemarie Pieper plädiert für ein Leben in Freiheit – und macht höchstpersönlich vor, wie Selbstbestimmung geht Sie war die erste Philosophin auf einem Lehrstuhl in Basel.
@@ -90,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,24 +151,37 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -213,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +255,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +307,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,14 +500,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,70 +532,59 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>